<commit_message>
slight function and folder modification
</commit_message>
<xml_diff>
--- a/expenses_record.xlsx
+++ b/expenses_record.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,16 +458,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2022-01-06</t>
+          <t>2022-01-08</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>120.09</v>
+        <v>150.25</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -478,116 +478,116 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2022-01-07</t>
+          <t>2022-01-09</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>156.41</v>
+        <v>41.05</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2022-01-07</t>
+          <t>2022-01-15</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>430.05</v>
+        <v>164.43</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2022-01-08</t>
+          <t>2022-01-16</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>121.21</v>
+        <v>229.2</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2022-01-10</t>
+          <t>2022-01-17</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>50.93</v>
+        <v>399.11</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2022-01-13</t>
+          <t>2022-01-21</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>409.69</v>
+        <v>30.5</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2022-01-15</t>
+          <t>2022-01-23</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>167.2</v>
+        <v>419.48</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -598,196 +598,196 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2022-01-15</t>
+          <t>2022-01-24</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>10.73</v>
+        <v>398.97</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2022-01-16</t>
+          <t>2022-01-30</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>358.69</v>
+        <v>262.26</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2022-01-26</t>
+          <t>2022-02-02</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>195.3</v>
+        <v>368.43</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2022-01-28</t>
+          <t>2022-02-02</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>404.02</v>
+        <v>250.82</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2022-01-30</t>
+          <t>2022-02-02</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>176.95</v>
+        <v>58.6</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Peter Joy</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2022-01-30</t>
+          <t>2022-02-02</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>398.53</v>
+        <v>145</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2022-01-31</t>
+          <t>2022-02-03</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>287.41</v>
+        <v>25.71</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2022-02-01</t>
+          <t>2022-02-05</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>414.81</v>
+        <v>144.42</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2022-02-02</t>
+          <t>2022-02-09</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>9.529999999999999</v>
+        <v>264.09</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2022-02-02</t>
+          <t>2022-02-16</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>121.28</v>
+        <v>297.22</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -798,60 +798,60 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2022-02-04</t>
+          <t>2022-02-18</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>124.04</v>
+        <v>47.87</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2022-02-15</t>
+          <t>2022-02-22</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>24.76</v>
+        <v>391.54</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2022-02-18</t>
+          <t>2022-03-01</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>114.48</v>
+        <v>53.12</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
@@ -863,75 +863,75 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2022-02-18</t>
+          <t>2022-03-01</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>319.42</v>
+        <v>229.77</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2022-02-19</t>
+          <t>2022-03-02</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>175.47</v>
+        <v>421.38</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2022-02-22</t>
+          <t>2022-03-09</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>258.4</v>
+        <v>206.75</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2022-02-26</t>
+          <t>2022-03-11</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>159.62</v>
+        <v>125.02</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
@@ -943,251 +943,251 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2022-02-28</t>
+          <t>2022-03-15</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>436.03</v>
+        <v>161.77</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2022-03-01</t>
+          <t>2022-03-17</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>41.19</v>
+        <v>372.2</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2022-03-07</t>
+          <t>2022-03-18</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>49.11</v>
+        <v>53.16</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2022-03-08</t>
+          <t>2022-03-24</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>28.19</v>
+        <v>325.14</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2022-03-14</t>
+          <t>2022-03-28</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>64.34999999999999</v>
+        <v>154.39</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2022-03-17</t>
+          <t>2022-04-04</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>201.09</v>
+        <v>1.28</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2022-03-17</t>
+          <t>2022-04-04</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>359.82</v>
+        <v>330.37</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2022-03-22</t>
+          <t>2022-04-05</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>6.76</v>
+        <v>111.41</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2022-03-24</t>
+          <t>2022-04-06</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>410.25</v>
+        <v>67.70999999999999</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2022-03-25</t>
+          <t>2022-04-07</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>189.58</v>
+        <v>306.32</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2022-03-27</t>
+          <t>2022-04-15</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>197.16</v>
+        <v>58.83</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2022-03-28</t>
+          <t>2022-04-17</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>31.03</v>
+        <v>55.12</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2022-04-03</t>
+          <t>2022-04-19</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>227.36</v>
+        <v>285.28</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1198,156 +1198,156 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2022-04-04</t>
+          <t>2022-04-29</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>388.81</v>
+        <v>406.28</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2022-04-05</t>
+          <t>2022-04-30</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>213.76</v>
+        <v>69.13</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2022-04-05</t>
+          <t>2022-05-03</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>408.59</v>
+        <v>60.41</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2022-04-11</t>
+          <t>2022-05-05</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>101.55</v>
+        <v>130.25</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2022-04-13</t>
+          <t>2022-05-05</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>412.52</v>
+        <v>281.74</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2022-04-18</t>
+          <t>2022-05-06</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>50.05</v>
+        <v>51.9</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2022-04-19</t>
+          <t>2022-05-16</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>372.05</v>
+        <v>65.26000000000001</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2022-04-20</t>
+          <t>2022-05-17</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>418.18</v>
+        <v>438.88</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1358,16 +1358,16 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2022-04-21</t>
+          <t>2022-05-17</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>386.21</v>
+        <v>164.73</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1378,80 +1378,80 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2022-04-22</t>
+          <t>2022-05-18</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>330.17</v>
+        <v>124.23</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2022-04-26</t>
+          <t>2022-05-23</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>123.56</v>
+        <v>213.4</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2022-04-26</t>
+          <t>2022-05-23</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>189.29</v>
+        <v>36.33</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2022-05-02</t>
+          <t>2022-05-25</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>376.02</v>
+        <v>420.48</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
@@ -1463,51 +1463,51 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2022-05-02</t>
+          <t>2022-05-25</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>322.25</v>
+        <v>303.96</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2022-05-06</t>
+          <t>2022-05-27</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>79.13</v>
+        <v>284.14</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2022-05-10</t>
+          <t>2022-05-27</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>308.37</v>
+        <v>29</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1518,36 +1518,36 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2022-05-15</t>
+          <t>2022-05-28</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>284.95</v>
+        <v>78.89</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2022-05-16</t>
+          <t>2022-06-02</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>333.71</v>
+        <v>405.03</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1558,40 +1558,40 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2022-05-23</t>
+          <t>2022-06-05</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>339.1</v>
+        <v>17.35</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2022-05-23</t>
+          <t>2022-06-08</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>43.85</v>
+        <v>193.01</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
@@ -1603,11 +1603,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2022-05-26</t>
+          <t>2022-06-13</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>146.93</v>
+        <v>443.83</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1618,36 +1618,36 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2022-05-31</t>
+          <t>2022-06-18</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>138.49</v>
+        <v>162.75</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2022-06-07</t>
+          <t>2022-06-20</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>260.99</v>
+        <v>103.2</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -1658,20 +1658,20 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2022-06-18</t>
+          <t>2022-06-22</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>291.02</v>
+        <v>264.25</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
@@ -1683,55 +1683,55 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2022-06-21</t>
+          <t>2022-06-28</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>363.91</v>
+        <v>110.81</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2022-06-25</t>
+          <t>2022-07-02</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>349.82</v>
+        <v>61.18</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2022-06-26</t>
+          <t>2022-07-06</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>441.87</v>
+        <v>243.75</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>party</t>
         </is>
       </c>
     </row>
@@ -1743,15 +1743,15 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2022-06-27</t>
+          <t>2022-07-09</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>182.7</v>
+        <v>115.71</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
@@ -1763,115 +1763,115 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2022-07-03</t>
+          <t>2022-07-11</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>234.31</v>
+        <v>359.69</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2022-07-05</t>
+          <t>2022-07-13</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>416.06</v>
+        <v>268.42</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2022-07-07</t>
+          <t>2022-07-14</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>401.25</v>
+        <v>14.11</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2022-07-11</t>
+          <t>2022-07-14</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>214.04</v>
+        <v>24.45</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2022-07-14</t>
+          <t>2022-07-17</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>379.66</v>
+        <v>183.3</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2022-07-16</t>
+          <t>2022-07-18</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>323.87</v>
+        <v>100.66</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
@@ -1883,71 +1883,71 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2022-07-16</t>
+          <t>2022-07-21</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>421.67</v>
+        <v>168.9</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2022-07-17</t>
+          <t>2022-07-22</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>432.33</v>
+        <v>352.07</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2022-07-19</t>
+          <t>2022-07-31</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>276.61</v>
+        <v>172.7</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-07-31</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>111.46</v>
+        <v>213.63</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -1958,60 +1958,60 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2022-07-28</t>
+          <t>2022-08-10</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>286.97</v>
+        <v>311.91</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2022-07-29</t>
+          <t>2022-08-15</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>165.11</v>
+        <v>328.04</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>2022-08-03</t>
+          <t>2022-08-22</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>25.72</v>
+        <v>45.12</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>party</t>
         </is>
       </c>
     </row>
@@ -2023,55 +2023,55 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>2022-08-04</t>
+          <t>2022-08-24</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>98.02</v>
+        <v>232.43</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2022-08-07</t>
+          <t>2022-08-26</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>180.95</v>
+        <v>368.99</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2022-08-09</t>
+          <t>2022-08-27</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>439.47</v>
+        <v>321.28</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>party</t>
         </is>
       </c>
     </row>
@@ -2083,15 +2083,15 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2022-08-21</t>
+          <t>2022-08-28</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>11.4</v>
+        <v>297.04</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
@@ -2103,31 +2103,31 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>2022-08-23</t>
+          <t>2022-08-30</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>37.52</v>
+        <v>380.83</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>2022-08-26</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>215.92</v>
+        <v>375.39</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -2143,55 +2143,55 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>2022-08-29</t>
+          <t>2022-09-08</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>33.94</v>
+        <v>307.05</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>2022-09-04</t>
+          <t>2022-09-15</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>63.3</v>
+        <v>11.04</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>2022-09-05</t>
+          <t>2022-09-19</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>199.4</v>
+        <v>49.27</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>party</t>
+          <t>transport</t>
         </is>
       </c>
     </row>
@@ -2203,55 +2203,55 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>2022-09-08</t>
+          <t>2022-09-20</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>127.14</v>
+        <v>217.55</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>James Kingsley</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>2022-09-11</t>
+          <t>2022-09-23</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>387.97</v>
+        <v>407.7</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>2022-09-12</t>
+          <t>2022-09-27</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>274.4</v>
+        <v>11.02</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
@@ -2263,11 +2263,11 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>2022-09-14</t>
+          <t>2022-09-30</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>374.2</v>
+        <v>416.52</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2278,16 +2278,16 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Saba Angella</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>2022-09-17</t>
+          <t>2022-10-04</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>317.43</v>
+        <v>440.76</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -2303,55 +2303,55 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>2022-09-18</t>
+          <t>2022-10-04</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>158.46</v>
+        <v>136.05</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>2022-09-19</t>
+          <t>2022-10-06</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>5.15</v>
+        <v>292.16</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Peter James</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>2022-09-20</t>
+          <t>2022-10-09</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>16.13</v>
+        <v>231.92</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
@@ -2363,75 +2363,75 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>2022-09-25</t>
+          <t>2022-10-10</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>368.16</v>
+        <v>343.24</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>2022-09-28</t>
+          <t>2022-10-13</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>392.02</v>
+        <v>272.21</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>2022-10-01</t>
+          <t>2022-10-17</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>119.33</v>
+        <v>344.71</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>2022-10-11</t>
+          <t>2022-10-18</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>65.95999999999999</v>
+        <v>34.66</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
@@ -2443,11 +2443,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>2022-10-13</t>
+          <t>2022-10-19</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>181.44</v>
+        <v>139.01</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -2458,20 +2458,20 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>2022-10-13</t>
+          <t>2022-10-24</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>413.7</v>
+        <v>73.59</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>party</t>
         </is>
       </c>
     </row>
@@ -2483,82 +2483,82 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>2022-10-13</t>
+          <t>2022-10-24</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>293.19</v>
+        <v>235.14</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>2022-10-21</t>
+          <t>2022-10-25</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>397.02</v>
+        <v>427.34</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>2022-10-29</t>
+          <t>2022-10-28</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>85.73999999999999</v>
+        <v>31.72</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>2022-10-31</t>
+          <t>2022-10-30</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>245.65</v>
+        <v>21.81</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Muhamed Sani</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -2567,91 +2567,91 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>26.35</v>
+        <v>197.81</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Mahar Schmidt</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>2022-11-04</t>
+          <t>2022-11-03</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>422.6</v>
+        <v>380.46</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>2022-11-06</t>
+          <t>2022-11-03</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>348.14</v>
+        <v>366.47</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>party</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>2022-11-14</t>
+          <t>2022-11-09</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>206.63</v>
+        <v>196.1</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>grocery</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Jonny Udoh</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>2022-11-20</t>
+          <t>2022-11-16</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>109.75</v>
+        <v>334.4</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>charity</t>
+          <t>party</t>
         </is>
       </c>
     </row>
@@ -2663,95 +2663,95 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>2022-11-21</t>
+          <t>2022-11-17</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>111.44</v>
+        <v>367.28</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>grocery</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Muhamed Sani</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>2022-11-27</t>
+          <t>2022-11-22</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>96.08</v>
+        <v>312.59</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Jonny Trump</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>2022-11-28</t>
+          <t>2022-11-25</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>113.03</v>
+        <v>137.38</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>cosmetic</t>
+          <t>insurance</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>2022-11-28</t>
+          <t>2022-12-03</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>35.12</v>
+        <v>105.79</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Mahar Schmidt</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>2022-12-09</t>
+          <t>2022-12-05</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>334.57</v>
+        <v>124.71</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
@@ -2763,95 +2763,115 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>2022-12-11</t>
+          <t>2022-12-07</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>338.41</v>
+        <v>212.92</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Barack Ade</t>
+          <t>Saba Angella</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>2022-12-11</t>
+          <t>2022-12-07</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>405.01</v>
+        <v>417.64</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>misc</t>
+          <t>charity</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>James Kingsley</t>
+          <t>Barack Ade</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>2022-12-12</t>
+          <t>2022-12-10</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>338.95</v>
+        <v>445.82</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>cosmetic</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Jonny Udoh</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>2022-12-13</t>
+          <t>2022-12-26</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>291.48</v>
+        <v>129.65</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>insurance</t>
+          <t>clothing</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Jonny Trump</t>
+          <t>Peter James</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>2022-12-19</t>
+          <t>2022-12-28</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>9.460000000000001</v>
+        <v>3.07</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>clothing</t>
+          <t>grocery</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Muhamed Sani</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>2022-12-31</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>201.57</v>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>misc</t>
         </is>
       </c>
     </row>

</xml_diff>